<commit_message>
New regex before calculating scores
</commit_message>
<xml_diff>
--- a/results/postprocessed/Modified_Outputs.xlsx
+++ b/results/postprocessed/Modified_Outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serenekim/Desktop/PhD/img-analysis_seorin_project/results/postprocessed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D713DC4D-5793-C641-B6B0-1FAAE87D55DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3F4F8A-157F-3746-B262-69012DF48E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{5EB31E44-82E6-F64F-B412-665BA69423F3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -251,10 +251,22 @@
     <t>Droits de Succession perçus 1920 [signature]</t>
   </si>
   <si>
-    <t>Claude_complex_perline_output2.csv</t>
-  </si>
-  <si>
     <t>Changed outputs due to “The image shows a handwritten…..” even after post-processing</t>
+  </si>
+  <si>
+    <t>Whole-scan</t>
+  </si>
+  <si>
+    <t>"Here's the recreated content of the table from the image: Arrêté le vingt cinq janvier 1920 Demarche servais 10² vingt six janvier Deflandre Gustave Désiré Tubize 22 8b 1919 Dubblemanns Delphine 898 510 - 107/1919 - - 10³ d Ypersiel Julien Ghislain Nivelles 15 8b 1918 Elexance Célestin 250 - 250 150/1919 - - Arrêté le vingt six janvier 1920 servais 10⁴ vingt sept janvier Cordeur Louis Braine l'Alleud 21 janvier 1919 Cordeur Antoine 300 - 300 111/1919 - - 27 janvier 1920 Arrêté le vingt sept janvier 1920 servais 10⁵ vingt huit janvier Decock Léonie Tubize 22 février 1919 Meuris David - 586 586 121/1920 - - 10⁶ d Decock Adèle - 10 8b 1915 - - - - 122/1920 - - 11 d Delendries Anastasie Nivelles 12 7b 1919 Delendries Delphine 1590 1395 195 - 11 mars 1920 8 avril 1920 Sommier 1920 169 Arrêté le vingt huit janvier 1920 servais Arrêté le vingt neuf janvier 1920 servais 11² trente janvier Rousseau Charles Gn Nivelles 18 mars 1919 Rousseau Louis 1500 - 1500 123/1919 - - 11³ d Dedoncker Vital Tubize 22 7b 1919 Brassemans Léocadie 4687 1536 3151 124/1919 - -"</t>
+  </si>
+  <si>
+    <t>"Arrêté le vingt cinq janvier 1920 Demarche servais 10² vingt six janvier Deflandre Gustave Désiré Tubize 22 8b 1919 Dubblemanns Delphine 898 510 - 107/1919 - - 10³ d Ypersiel Julien Ghislain Nivelles 15 8b 1918 Elexance Célestin 250 - 250 150/1919 - - Arrêté le vingt six janvier 1920 servais 10⁴ vingt sept janvier Cordeur Louis Braine l'Alleud 21 janvier 1919 Cordeur Antoine 300 - 300 111/1919 - - 27 janvier 1920 Arrêté le vingt sept janvier 1920 servais 10⁵ vingt huit janvier Decock Léonie Tubize 22 février 1919 Meuris David - 586 586 121/1920 - - 10⁶ d Decock Adèle - 10 8b 1915 - - - - 122/1920 - - 11 d Delendries Anastasie Nivelles 12 7b 1919 Delendries Delphine 1590 1395 195 - 11 mars 1920 8 avril 1920 Sommier 1920 169 Arrêté le vingt huit janvier 1920 servais Arrêté le vingt neuf janvier 1920 servais 11² trente janvier Rousseau Charles Gn Nivelles 18 mars 1919 Rousseau Louis 1500 - 1500 123/1919 - - 11³ d Dedoncker Vital Tubize 22 7b 1919 Brassemans Léocadie 4687 1536 3151 124/1919 - -"</t>
+  </si>
+  <si>
+    <t>claude_one_example_whole_output.csv // new_transcription16.txt</t>
+  </si>
+  <si>
+    <t>Example 17 // ID 16</t>
   </si>
 </sst>
 </file>
@@ -670,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0109394F-3307-174D-B497-DA29ACD24312}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="134" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,7 +699,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -884,7 +896,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -901,7 +913,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -952,7 +964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -1088,52 +1100,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="221" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>4</v>
+        <v>75</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>